<commit_message>
ouaip - return vide si non trouvé
</commit_message>
<xml_diff>
--- a/Table VN Boulpat.xlsx
+++ b/Table VN Boulpat.xlsx
@@ -253,7 +253,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -263,12 +263,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,14 +279,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -590,7 +583,7 @@
   <dimension ref="A1:BR1793"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="L14" sqref="L13:L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
@@ -879,7 +872,9 @@
       <c r="I3" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="J3" s="4"/>
+      <c r="J3" s="2">
+        <v>1514</v>
+      </c>
       <c r="K3" s="2">
         <v>361</v>
       </c>
@@ -939,7 +934,9 @@
       <c r="I4" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J4" s="4"/>
+      <c r="J4" s="2">
+        <v>1335</v>
+      </c>
       <c r="K4" s="2">
         <v>318</v>
       </c>

</xml_diff>

<commit_message>
boucle Energie de ciqual_import, tests pour validation
</commit_message>
<xml_diff>
--- a/Table VN Boulpat.xlsx
+++ b/Table VN Boulpat.xlsx
@@ -582,8 +582,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:BR1793"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L14" sqref="L13:L14"/>
+    <sheetView tabSelected="1" topLeftCell="BH1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <pane xSplit="15210" topLeftCell="Q1"/>
+      <selection activeCell="X2" sqref="X2"/>
+      <selection pane="topRight" activeCell="Q1" sqref="Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="12.75"/>
@@ -628,6 +630,15 @@
       <c r="U1" s="3">
         <v>34100</v>
       </c>
+      <c r="V1" s="3">
+        <v>34000</v>
+      </c>
+      <c r="X1" s="3">
+        <v>60000</v>
+      </c>
+      <c r="Y1" s="3">
+        <v>65000</v>
+      </c>
       <c r="Z1" s="3">
         <v>40302</v>
       </c>

</xml_diff>